<commit_message>
analiza danych 310725 2
</commit_message>
<xml_diff>
--- a/pomiary/pomiary_230725/kalibracja/krzywa kalibracyjna.xlsx
+++ b/pomiary/pomiary_230725/kalibracja/krzywa kalibracyjna.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Lab 142\Osobiste\Julia\krzywa kalibracyjna 23072025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gosc\Desktop\Rezonatory2025\Rezonatory2025\pomiary\pomiary_230725\kalibracja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40788DE-649F-4342-A5E0-E57FC401A333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C069BF40-0A7A-4D25-8DBC-8D6387A96326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AC994A45-B5C3-41A3-90F0-38B0A4590F74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AC994A45-B5C3-41A3-90F0-38B0A4590F74}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -1464,6 +1464,1190 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Szerokość X [um]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz2!$A$2:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>34.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>35.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>36.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>38.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz2!$B$2:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1060</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>918</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>834</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>794</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>738</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>707</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>651</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>607</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>506</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>374</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>88.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>75.8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>73.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>77.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>86.8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>351</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>394</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>436</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>484</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>536</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>632</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>685</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>734</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>787</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DCFF-4004-B036-FC3EB273F65F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1500769216"/>
+        <c:axId val="1500771616"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1500769216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1500771616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1500771616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1500769216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Arkusz2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Szerokość Y [um]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Arkusz2!$A$2:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>34.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>35.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>36.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>38.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Arkusz2!$C$2:$C$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>1325</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1201</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1080</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1040</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>978</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>951</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>827</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>771</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>657</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>608</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>556</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>522</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>453</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>102.8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>83.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>69.8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>67.3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>73.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>85.7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>376</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>433</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>482</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>536</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>589</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>639</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>689</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>753</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>799</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>866</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0A21-404C-9089-D4F16CDE3742}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1500767296"/>
+        <c:axId val="1500767776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1500767296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1500767776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1500767776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1500767296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pl-PL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1544,6 +2728,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2061,6 +3325,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2653,10 +4949,87 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90D49279-7217-E99F-17F2-4B9122FB63D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD20988A-A03E-342E-50E8-6CBC88AC5DE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Pakiet Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2694,7 +5067,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Pakiet Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2800,7 +5173,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Pakiet Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2942,7 +5315,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3617,7 +5990,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCellId="1" sqref="C1:C1048576 A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4179,5 +6552,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>